<commit_message>
Kuksu: generate group-player correspondences
</commit_message>
<xml_diff>
--- a/past_performance.xlsx
+++ b/past_performance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>IcedEarth</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>nomadfarmer</t>
+  </si>
+  <si>
+    <t>tzorec</t>
   </si>
 </sst>
 </file>
@@ -512,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -536,80 +539,80 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="B2">
-        <v>667</v>
+        <v>120</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
-        <v>870</v>
+        <v>667</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>913</v>
+        <v>870</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>1647</v>
+        <v>913</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>1707</v>
+        <v>1647</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
-        <v>2394</v>
+        <v>1707</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -620,13 +623,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>3503</v>
+        <v>2394</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -634,66 +637,66 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>3710</v>
+        <v>3503</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>4048</v>
+        <v>3710</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>5093</v>
+        <v>4048</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>5832</v>
+        <v>5093</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>10377</v>
+        <v>5832</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -704,139 +707,139 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>11332</v>
+        <v>10377</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>12573</v>
+        <v>11332</v>
       </c>
       <c r="C15">
         <v>5</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16">
-        <v>13916</v>
+        <v>12573</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17">
-        <v>14124</v>
+        <v>13916</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18">
-        <v>15530</v>
+        <v>14124</v>
       </c>
       <c r="C18">
         <v>4</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19">
-        <v>16805</v>
+        <v>15530</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>24005</v>
+        <v>16805</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21">
-        <v>27500</v>
+        <v>24005</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22">
-        <v>28201</v>
+        <v>27500</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23">
-        <v>30316</v>
+        <v>28201</v>
       </c>
       <c r="C23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -844,13 +847,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24">
-        <v>31101</v>
+        <v>30316</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>2</v>
@@ -858,94 +861,94 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25">
-        <v>31287</v>
+        <v>31101</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26">
-        <v>31467</v>
+        <v>31287</v>
       </c>
       <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
         <v>1</v>
-      </c>
-      <c r="D26">
-        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27">
-        <v>31958</v>
+        <v>31467</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28">
-        <v>33380</v>
+        <v>31958</v>
       </c>
       <c r="C28">
         <v>5</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29">
-        <v>34056</v>
+        <v>33380</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>34541</v>
+        <v>34056</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B31">
-        <v>34917</v>
+        <v>34541</v>
       </c>
       <c r="C31">
         <v>3</v>
@@ -956,13 +959,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32">
-        <v>36843</v>
+        <v>34917</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -970,223 +973,223 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33">
-        <v>37174</v>
+        <v>36843</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34">
-        <v>37357</v>
+        <v>37174</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35">
-        <v>37721</v>
+        <v>37357</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36">
-        <v>37892</v>
+        <v>37721</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37">
-        <v>37952</v>
+        <v>37892</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D37">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38">
-        <v>39317</v>
+        <v>37952</v>
       </c>
       <c r="C38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D38">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39">
-        <v>39360</v>
+        <v>39317</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40">
-        <v>40318</v>
+        <v>39360</v>
       </c>
       <c r="C40">
         <v>2</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B41">
-        <v>41015</v>
+        <v>40318</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B42">
-        <v>41020</v>
+        <v>41015</v>
       </c>
       <c r="C42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B43">
-        <v>41805</v>
+        <v>41020</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D43">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B44">
-        <v>42542</v>
+        <v>41805</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B45">
-        <v>43936</v>
+        <v>42542</v>
       </c>
       <c r="C45">
         <v>2</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46">
-        <v>45330</v>
+        <v>43936</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47">
-        <v>45528</v>
+        <v>45330</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B48">
-        <v>46488</v>
+        <v>45528</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D48">
         <v>2</v>
@@ -1194,15 +1197,29 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49">
+        <v>46488</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
         <v>45</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>46653</v>
       </c>
-      <c r="C49">
-        <v>5</v>
-      </c>
-      <c r="D49">
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="D50">
         <v>5</v>
       </c>
     </row>

</xml_diff>